<commit_message>
Implement form change req
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_death/forms/hh_death/hh_death.xlsx
+++ b/odkx/app/config/tables/hh_death/forms/hh_death/hh_death.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="123">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -54,9 +54,6 @@
     <t xml:space="preserve">display.prompt</t>
   </si>
   <si>
-    <t xml:space="preserve">display.hint.text</t>
-  </si>
-  <si>
     <t xml:space="preserve">inputAttributes.min</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
   </si>
   <si>
     <t xml:space="preserve">q65a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC-123-700</t>
   </si>
   <si>
     <t xml:space="preserve">/^[A-Z]{3}-[0-9]{3}-7[0-9]{2}$/.test(data('hh_death_id'))</t>
@@ -506,7 +500,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
@@ -546,13 +540,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.83"/>
@@ -560,13 +554,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="43.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="43.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,179 +599,173 @@
       <c r="L1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="K5" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="K9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" s="0" t="n">
+      <c r="L9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="M11" s="0" t="n">
+      <c r="L11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>52</v>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -803,7 +790,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.39"/>
@@ -812,46 +799,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -876,7 +863,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.39"/>
@@ -892,58 +879,58 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -964,11 +951,11 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.47"/>
@@ -980,41 +967,41 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20210221001</v>
@@ -1022,79 +1009,79 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -1122,7 +1109,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="38.88"/>
@@ -1130,198 +1117,198 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>86</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement change requests for forms
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_death/forms/hh_death/hh_death.xlsx
+++ b/odkx/app/config/tables/hh_death/forms/hh_death/hh_death.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="123">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -72,24 +72,24 @@
     <t xml:space="preserve">hideInContents</t>
   </si>
   <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_death_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q65a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/^[A-Z]{3}-[0-9]{3}-7[0-9]{2}$/.test(data('hh_death_id'))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extid_format</t>
+  </si>
+  <si>
     <t xml:space="preserve">begin screen</t>
   </si>
   <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_death_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q65a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/^[A-Z]{3}-[0-9]{3}-7[0-9]{2}$/.test(data('hh_death_id'))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extid_format</t>
-  </si>
-  <si>
     <t xml:space="preserve">hh_death_name</t>
   </si>
   <si>
@@ -114,6 +114,9 @@
     <t xml:space="preserve">surname_number</t>
   </si>
   <si>
+    <t xml:space="preserve">end screen</t>
+  </si>
+  <si>
     <t xml:space="preserve">select_one</t>
   </si>
   <si>
@@ -178,9 +181,6 @@
   </si>
   <si>
     <t xml:space="preserve">q65f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end screen</t>
   </si>
   <si>
     <t xml:space="preserve">choice_list_name</t>
@@ -500,7 +500,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
@@ -540,13 +540,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.83"/>
@@ -601,30 +601,30 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="0" t="s">
+      <c r="A3" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>21</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>25</v>
@@ -657,66 +657,57 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="s">
+      <c r="A6" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>1</v>
@@ -724,48 +715,67 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>51</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -790,7 +800,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.39"/>
@@ -810,7 +820,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>55</v>
@@ -821,7 +831,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>56</v>
@@ -832,13 +842,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -863,7 +873,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.39"/>
@@ -887,10 +897,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -898,7 +908,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,31 +916,31 @@
         <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -951,11 +961,11 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.47"/>
@@ -1004,7 +1014,7 @@
         <v>69</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>20210221001</v>
+        <v>20210304001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,7 +1044,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1109,7 +1119,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="38.88"/>
@@ -1120,7 +1130,7 @@
         <v>81</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>82</v>
@@ -1131,7 +1141,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>84</v>
@@ -1173,7 +1183,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>93</v>
@@ -1187,7 +1197,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>96</v>
@@ -1201,7 +1211,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>99</v>
@@ -1215,7 +1225,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>102</v>
@@ -1285,7 +1295,7 @@
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>117</v>
@@ -1299,7 +1309,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>120</v>

</xml_diff>